<commit_message>
Add row trabajos in Rtech and format 24 hrs in dates
</commit_message>
<xml_diff>
--- a/ReportTechOut.xlsx
+++ b/ReportTechOut.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="85">
   <si>
     <t>INFORME TECNICO</t>
   </si>
@@ -249,6 +249,9 @@
   <si>
     <t>Mantenimiento /
 Inspecciones</t>
+  </si>
+  <si>
+    <t>kalza</t>
   </si>
   <si>
     <t>Sujerancias /
@@ -43821,7 +43824,9 @@
       <c r="E22" s="39"/>
       <c r="F22" s="39"/>
       <c r="G22" s="39"/>
-      <c r="H22" s="29"/>
+      <c r="H22" s="29" t="s">
+        <v>68</v>
+      </c>
       <c r="I22" s="29"/>
       <c r="J22" s="29"/>
       <c r="K22" s="29"/>
@@ -43951,7 +43956,7 @@
     <row r="25" spans="1:1025" customHeight="1" ht="12.75">
       <c r="A25" s="2"/>
       <c r="B25" s="39" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C25" s="39"/>
       <c r="D25" s="39"/>
@@ -43959,7 +43964,7 @@
       <c r="F25" s="39"/>
       <c r="G25" s="39"/>
       <c r="H25" s="29" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I25" s="29"/>
       <c r="J25" s="29"/>
@@ -46022,7 +46027,7 @@
       <c r="AL70" s="22"/>
       <c r="AM70" s="22"/>
       <c r="AN70" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="AO70" s="23"/>
       <c r="AP70" s="23"/>
@@ -47330,7 +47335,7 @@
     <row r="5" spans="1:1025" customHeight="1" ht="17.25">
       <c r="A5" s="2"/>
       <c r="B5" s="35" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C5" s="35"/>
       <c r="D5" s="35"/>
@@ -47338,7 +47343,7 @@
       <c r="F5" s="35"/>
       <c r="G5" s="35"/>
       <c r="H5" s="40" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I5" s="40"/>
       <c r="J5" s="40"/>
@@ -48087,12 +48092,12 @@
     <row r="22" spans="1:1025" customHeight="1" ht="11.25">
       <c r="A22" s="2"/>
       <c r="B22" s="24" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C22" s="24"/>
       <c r="D22" s="24"/>
       <c r="E22" s="25" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="F22" s="25"/>
       <c r="G22" s="25"/>
@@ -48110,11 +48115,11 @@
       <c r="S22" s="25"/>
       <c r="T22" s="25"/>
       <c r="U22" s="24" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="V22" s="24"/>
       <c r="W22" s="25" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="X22" s="25"/>
       <c r="Y22" s="25"/>
@@ -48843,7 +48848,7 @@
     <row r="39" spans="1:1025" customHeight="1" ht="15">
       <c r="A39" s="2"/>
       <c r="B39" s="24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C39" s="24"/>
       <c r="D39" s="24"/>
@@ -48866,7 +48871,7 @@
       <c r="S39" s="25"/>
       <c r="T39" s="25"/>
       <c r="U39" s="24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="V39" s="24"/>
       <c r="W39" s="25">
@@ -49599,7 +49604,7 @@
     <row r="56" spans="1:1025" customHeight="1" ht="17.25">
       <c r="A56" s="2"/>
       <c r="B56" s="24" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C56" s="24"/>
       <c r="D56" s="24"/>
@@ -49622,7 +49627,7 @@
       <c r="S56" s="25"/>
       <c r="T56" s="25"/>
       <c r="U56" s="24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="V56" s="24"/>
       <c r="W56" s="24"/>
@@ -50355,7 +50360,7 @@
     <row r="73" spans="1:1025" customHeight="1" ht="11.25">
       <c r="A73" s="2"/>
       <c r="B73" s="24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C73" s="24"/>
       <c r="D73" s="24"/>
@@ -50378,7 +50383,7 @@
       <c r="S73" s="25"/>
       <c r="T73" s="25"/>
       <c r="U73" s="24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="V73" s="24"/>
       <c r="W73" s="24"/>
@@ -50490,7 +50495,7 @@
       <c r="AJ75" s="22"/>
       <c r="AK75" s="22"/>
       <c r="AL75" s="23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AM75" s="23"/>
       <c r="AN75" s="23"/>

</xml_diff>